<commit_message>
Quase finalizando analisador sintatico
</commit_message>
<xml_diff>
--- a/tabelaProducoes.xlsx
+++ b/tabelaProducoes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26522"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01FDAA00-C538-4547-AB93-416083BCFDFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{231E5B60-C852-4D66-93B1-6519B490BB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
     <t>, IDS</t>
   </si>
   <si>
-    <t>se ( COND ) Entao Bloco CMD'</t>
+    <t>se ( COND ) entao Bloco CMD'</t>
   </si>
   <si>
     <t>ID = Expressao ;</t>
@@ -603,7 +603,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Ajustes finais analisador sintatico
</commit_message>
<xml_diff>
--- a/tabelaProducoes.xlsx
+++ b/tabelaProducoes.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26522"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{231E5B60-C852-4D66-93B1-6519B490BB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAA12BB1-920A-42B7-B966-144FCBE98BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
     <t>Producoes</t>
   </si>
   <si>
-    <t>function ID Bloco</t>
+    <t>function ID ( ) Bloco</t>
   </si>
   <si>
     <t>{ DeclaracaoVariavel Comandos }</t>
@@ -57,13 +57,13 @@
     <t>, IDS</t>
   </si>
   <si>
-    <t>se ( COND ) entao Bloco CMD'</t>
-  </si>
-  <si>
-    <t>ID = Expressao ;</t>
-  </si>
-  <si>
-    <t>enquanto ( Cond ) faca Bloco</t>
+    <t xml:space="preserve">se ( Cond ) entao Bloco CMD' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID = Expressao ; </t>
+  </si>
+  <si>
+    <t>enquanto ( Cond) faca Bloco</t>
   </si>
   <si>
     <t>repita Bloco ate ( Cond )</t>
@@ -78,10 +78,10 @@
     <t>Pre1 Expressao'</t>
   </si>
   <si>
-    <t>+  Pre1' Expressao</t>
-  </si>
-  <si>
-    <t>-  Pre1' Expressao'</t>
+    <t>+ Pre1 Expressao'</t>
+  </si>
+  <si>
+    <t>- Pre1 Expressao'</t>
   </si>
   <si>
     <t>Pre2 Pre1'</t>
@@ -114,16 +114,16 @@
     <t>&lt;=</t>
   </si>
   <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>&gt;=</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve"> ==</t>
-  </si>
-  <si>
-    <t>&lt;</t>
-  </si>
-  <si>
-    <t>&gt;</t>
-  </si>
-  <si>
-    <t>&gt;=</t>
   </si>
   <si>
     <t>char</t>
@@ -256,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -284,6 +284,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -602,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -699,7 +702,7 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="5"/>
@@ -756,7 +759,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -770,7 +773,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -784,7 +787,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -798,7 +801,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -812,7 +815,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -826,7 +829,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -840,7 +843,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -854,7 +857,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -868,7 +871,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -882,7 +885,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -896,7 +899,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -905,12 +908,12 @@
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" ht="15.75">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>18</v>
+      <c r="B22" s="11" t="s">
+        <v>4</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -924,7 +927,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -938,7 +941,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -952,17 +955,17 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" ht="15.75">
       <c r="A26" s="1">
         <v>25</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>21</v>
+      <c r="B26" s="11" t="s">
+        <v>4</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -972,7 +975,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -982,17 +985,17 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" ht="15.75">
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>23</v>
+      <c r="B29" s="11" t="s">
+        <v>4</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1002,7 +1005,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1012,7 +1015,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1022,7 +1025,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1032,7 +1035,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -1042,7 +1045,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1052,7 +1055,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -1062,7 +1065,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -1072,7 +1075,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -1082,7 +1085,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -1092,7 +1095,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -1102,7 +1105,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -1116,7 +1119,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajustando Aritmético e Cond )
</commit_message>
<xml_diff>
--- a/tabelaProducoes.xlsx
+++ b/tabelaProducoes.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26522"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAA12BB1-920A-42B7-B966-144FCBE98BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Vinício\UFU\7\CC\analisador-sintatico\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC07FDB-4626-46AA-B7CC-D523460D07BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -63,9 +68,6 @@
     <t xml:space="preserve">ID = Expressao ; </t>
   </si>
   <si>
-    <t>enquanto ( Cond) faca Bloco</t>
-  </si>
-  <si>
     <t>repita Bloco ate ( Cond )</t>
   </si>
   <si>
@@ -133,6 +135,9 @@
   </si>
   <si>
     <t>float</t>
+  </si>
+  <si>
+    <t>enquanto ( Cond ) faca Bloco</t>
   </si>
 </sst>
 </file>
@@ -307,7 +312,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -801,7 +806,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -815,7 +820,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -829,7 +834,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -857,7 +862,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
@@ -871,7 +876,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -885,7 +890,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -899,7 +904,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
@@ -927,7 +932,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -941,7 +946,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -955,7 +960,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -975,7 +980,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -985,7 +990,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -1005,7 +1010,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1015,7 +1020,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -1025,7 +1030,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1035,7 +1040,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -1045,7 +1050,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1055,7 +1060,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -1065,7 +1070,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -1075,7 +1080,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -1085,7 +1090,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -1095,7 +1100,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -1105,7 +1110,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
@@ -1119,7 +1124,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>